<commit_message>
Correction de l'évaluation des compétance
</commit_message>
<xml_diff>
--- a/FichesTemps/EvalElementsDeCompetences.xlsx
+++ b/FichesTemps/EvalElementsDeCompetences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cegep\Session 6\Projet\Rooftop\FichesTemps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0921DFCB-F6B7-4760-87D4-1104E3E323D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C464FD0-8E3E-43DA-BE60-A39F76174878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,28 +395,10 @@
     <t>Grand total</t>
   </si>
   <si>
-    <t>La documentation et le découpage fonctionnel de notre projet a été, à notre humble avis, très bien effectué. Cependant, la gestion de temps fut somme toute inefficace. Les durées associées aux cas d'utilisations étaient inadéquates. Il y a eu un manque de compréhension de notre part. Durant notre parcours collégial, nous étions habitués à planifier des durées par cas d'utilisations. Cependant, dans un contexte comme celui-ci, il aurait été plus pertinent de planifier par semaine.</t>
-  </si>
-  <si>
-    <t>Nous aurions pu trouver un outil qui génère la documentation pour notre API, cela nous aurais permis d'avoir de la documentation programmeur directement lié au code qui nécessiterait moins de temps à maintenir.</t>
-  </si>
-  <si>
     <t>Puisque notre documentation est sous format .docx, elle n'a pas un bon format pour être disponible en ligne. Cependant ce n'est pas difficile à changer en .pdf</t>
   </si>
   <si>
-    <t>Comme écrit plus haut l'estimation du temps requis pour les cas d'utilisation n'a pas été très réaliste, ainsi beaucoup de tâches ont excéder le temps requis à chaque semaine et d'autres ont prit beaucoup moins de temps à chaque semaine. De plus, puisque l'estimation n'était pas réaliste, alors l'échéancier de travail a été très difficile à suivre à cause du temps qui était iréaliste.</t>
-  </si>
-  <si>
     <t>Nous n'avons pas assez vérifié le code de nos coéquipiers, cela aurait été facile à faire avec des pulls requests et des branches du git. Cela pourrait potentiellement causer une baisse de qualité du code à certains endroits.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nous avons créé un document détaillé pour expliquer clairement l'utilisation du logiciel par n'importe quel type d'utilisateur. Lors de la démonstration de l'application à la cliente, nous avons pu observé l'un de ces utilisateurs finaux intéragir avec notre application et ainsi connaître la profondeur et les aspects à couvrir dans notre document de formation. Nous sommes donc confiant qu'il convient à ceux-ci.  </t>
-  </si>
-  <si>
-    <t>Nous avons placé nos fichiers dans des fichiers qui ont du sens (exemple la documentation dans le fichier docs) avec une structure vu dans le cour de génie 1. Il est donc facile de se retrouver. Donc nous pensons donc que c'est l'archivage des documents est bien fait.</t>
-  </si>
-  <si>
-    <t>Nous aurions pu mieux utiliser la méthodologie de travail "AGILE" pour mieux gérer nos cycles de développement. Par exemple, on aurait pu faire plus de rencontres AGILE et plus réviser le code de nos pairs pour produire un code plus homogène et simple à comprendre. En général, nous avons bien suivis nos devis de développement, mais quelque fois le temps pris pour faire certains développement était plus long que prévu, ainsi nous aurrions pu mieux prévoir le dévelopement de l'application.</t>
   </si>
   <si>
     <t>Nous avons bien communiqué tout au long du développement entre nous (sur discord, en présence et sur notre Trello), pour résoudre les problèmes qui survenaient. Donc, au niveau de la communication, nous sommes satisfaits.</t>
@@ -456,6 +438,24 @@
   </si>
   <si>
     <t>Il aurait été mieux pour un client que la documentation soit disponible à partir de l'application, par exemple par un hyperlien. Cela aurait rendu la documentation plus accessible.</t>
+  </si>
+  <si>
+    <t>Nous aurions pu mieux utiliser la méthodologie de travail "AGILE" pour mieux gérer nos cycles de développement. Par exemple, on aurait pu faire plus de rencontres AGILE et plus réviser le code de nos pairs pour produire un code plus homogène et simple à comprendre. En général, nous avons bien suivi nos devis de développement, mais quelquefois le temps pris pour faire certains développements était plus long que prévu, ainsi nous aurions pu mieux prévoir le développement de l'application.</t>
+  </si>
+  <si>
+    <t>Comme écrit plus haut l'estimation du temps requis pour les cas d'utilisation n'a pas été très réaliste, ainsi beaucoup de tâches ont excédé le temps requis chaque semaine et d'autres ont pris beaucoup moins de temps chaque semaine. De plus, puisque l'estimation n'était pas réaliste, alors l'échéancier de travail a été très difficile à suivre à cause du temps qui était irréaliste.</t>
+  </si>
+  <si>
+    <t>Nous avons placé nos fichiers dans des fichiers qui ont du sens (exemple la documentation dans le fichier docs) avec une structure vue dans le cours de génie 1. Il est donc facile de se retrouver. Donc nous pensons donc que c'est l'archivage des documents est bien fait.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nous avons créé un document détaillé pour expliquer clairement l'utilisation du logiciel par n'importe quel type d'utilisateur. Lors de la démonstration de l'application à la cliente, nous avons pu observer l'un de ses utilisateurs finaux interagir avec notre application et ainsi connaître la profondeur et les aspects à couvrir dans notre document de formation. Nous sommes donc sûrs qu'il convient à ceux-ci.  </t>
+  </si>
+  <si>
+    <t>Nous aurions pu trouver un outil qui génère la documentation pour notre API, cela nous aurait permis d'avoir de la documentation programmeur directement lié au code qui nécessiterait moins de temps à maintenir.</t>
+  </si>
+  <si>
+    <t>La documentation et le découpage fonctionnel de notre projet ont été, à notre humble avis, très bien effectués. Cependant, la gestion de temps fut somme toute inefficace. Les durées associées aux cas d'utilisations étaient inadéquates. Il y a eu un manque de compréhension de notre part. Durant notre parcours collégial, nous étions habitués à planifier des durées par cas d'utilisations. Cependant, dans un contexte comme celui-ci, il aurait été plus pertinent de planifier par semaine.</t>
   </si>
 </sst>
 </file>
@@ -1069,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1115,20 +1115,20 @@
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="11" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C5" s="10">
         <v>0.05</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="11" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="21" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="12" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1222,7 +1222,7 @@
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1235,7 +1235,7 @@
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="13" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="11" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="146.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1277,7 +1277,7 @@
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="12" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1316,7 +1316,7 @@
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="13" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>